<commit_message>
dataset and prompts updated
</commit_message>
<xml_diff>
--- a/data/Bowling_against_left_right_handers.xlsx
+++ b/data/Bowling_against_left_right_handers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anees\MyCodingSpace\Text to CSV LLM with Pandas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C63202-62D5-40E3-A632-17FDA1281180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A21D9F-91BC-490D-AE47-CCAFEB862767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1375,9 +1375,6 @@
     <t>ball_bowled</t>
   </si>
   <si>
-    <t>matches played</t>
-  </si>
-  <si>
     <t>bowling_style</t>
   </si>
   <si>
@@ -1388,6 +1385,9 @@
   </si>
   <si>
     <t>bowling_strike_rate</t>
+  </si>
+  <si>
+    <t>matches_played</t>
   </si>
 </sst>
 </file>
@@ -1765,7 +1765,7 @@
   <dimension ref="A1:L575"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:XFD1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1790,22 +1790,22 @@
         <v>450</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>451</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>452</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">

</xml_diff>